<commit_message>
updated CSV files to OCT-15
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/purpose_processing.xlsx
+++ b/documentation-generator/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="845">
   <si>
     <t>Term</t>
   </si>
@@ -2438,6 +2438,24 @@
   </si>
   <si>
     <t>Processing that involves systematic monitoring of individuals</t>
+  </si>
+  <si>
+    <t>ProcessingCondition</t>
+  </si>
+  <si>
+    <t>Processing Condition</t>
+  </si>
+  <si>
+    <t>ProcessingLocation</t>
+  </si>
+  <si>
+    <t>Processing Location</t>
+  </si>
+  <si>
+    <t>ProcessingDuration</t>
+  </si>
+  <si>
+    <t>Processing Duration</t>
   </si>
   <si>
     <t>Scale</t>
@@ -32690,20 +32708,118 @@
       <c r="I45" s="91"/>
     </row>
     <row r="46">
-      <c r="A46" s="65"/>
-      <c r="B46" s="76"/>
+      <c r="A46" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>734</v>
+      </c>
       <c r="C46" s="98"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
       <c r="I46" s="91"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="8"/>
+      <c r="Y46" s="8"/>
+      <c r="Z46" s="8"/>
+      <c r="AA46" s="8"/>
+      <c r="AB46" s="8"/>
+      <c r="AC46" s="8"/>
+      <c r="AD46" s="8"/>
     </row>
     <row r="47">
-      <c r="B47" s="76"/>
+      <c r="A47" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>736</v>
+      </c>
       <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
       <c r="I47" s="91"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
+      <c r="V47" s="8"/>
+      <c r="W47" s="8"/>
+      <c r="X47" s="8"/>
+      <c r="Y47" s="8"/>
+      <c r="Z47" s="8"/>
+      <c r="AA47" s="8"/>
+      <c r="AB47" s="8"/>
+      <c r="AC47" s="8"/>
+      <c r="AD47" s="8"/>
     </row>
     <row r="48">
-      <c r="B48" s="76"/>
+      <c r="A48" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>738</v>
+      </c>
       <c r="C48" s="7"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
       <c r="I48" s="91"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="8"/>
+      <c r="W48" s="8"/>
+      <c r="X48" s="8"/>
+      <c r="Y48" s="8"/>
+      <c r="Z48" s="8"/>
+      <c r="AA48" s="8"/>
+      <c r="AB48" s="8"/>
+      <c r="AC48" s="8"/>
+      <c r="AD48" s="8"/>
     </row>
     <row r="49">
       <c r="B49" s="76"/>
@@ -37489,13 +37605,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>733</v>
+        <v>739</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>623</v>
@@ -37507,7 +37623,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="94" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="9">
@@ -37518,7 +37634,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>99</v>
@@ -37551,16 +37667,16 @@
     </row>
     <row r="4">
       <c r="A4" s="65" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>739</v>
+        <v>745</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>34</v>
@@ -37578,7 +37694,7 @@
         <v>22</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>99</v>
@@ -37599,16 +37715,16 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>18</v>
@@ -37647,16 +37763,16 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>746</v>
+        <v>752</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>18</v>
@@ -37695,16 +37811,16 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>749</v>
+        <v>755</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>756</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>750</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>744</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
@@ -37722,7 +37838,7 @@
         <v>22</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>99</v>
@@ -37743,16 +37859,16 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>752</v>
+        <v>758</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>753</v>
+        <v>759</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>18</v>
@@ -37791,16 +37907,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="C9" s="99" t="s">
-        <v>757</v>
+        <v>763</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>18</v>
@@ -37839,16 +37955,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>759</v>
+        <v>765</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
@@ -37899,16 +38015,16 @@
     </row>
     <row r="12">
       <c r="A12" s="65" t="s">
-        <v>761</v>
+        <v>767</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>762</v>
+        <v>768</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>763</v>
+        <v>769</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>34</v>
@@ -37926,7 +38042,7 @@
         <v>22</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="O12" s="10" t="s">
         <v>99</v>
@@ -37947,16 +38063,16 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>765</v>
+        <v>771</v>
       </c>
       <c r="C13" s="100" t="s">
-        <v>766</v>
+        <v>772</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
@@ -37995,16 +38111,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>768</v>
+        <v>774</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>769</v>
+        <v>775</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>770</v>
+        <v>776</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>18</v>
@@ -38043,16 +38159,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>771</v>
+        <v>777</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>779</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>773</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>767</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>18</v>
@@ -38070,7 +38186,7 @@
         <v>22</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="O15" s="10" t="s">
         <v>99</v>
@@ -38091,16 +38207,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>775</v>
+        <v>781</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>18</v>
@@ -38139,16 +38255,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>777</v>
+        <v>783</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>778</v>
+        <v>784</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>779</v>
+        <v>785</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>18</v>
@@ -38187,16 +38303,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>780</v>
+        <v>786</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>781</v>
+        <v>787</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>782</v>
+        <v>788</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
@@ -38247,16 +38363,16 @@
     </row>
     <row r="20">
       <c r="A20" s="65" t="s">
-        <v>783</v>
+        <v>789</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>784</v>
+        <v>790</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>785</v>
+        <v>791</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>34</v>
@@ -38274,7 +38390,7 @@
         <v>22</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="O20" s="10" t="s">
         <v>99</v>
@@ -38295,16 +38411,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>787</v>
+        <v>793</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>18</v>
@@ -38343,16 +38459,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>790</v>
+        <v>796</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>791</v>
+        <v>797</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>792</v>
+        <v>798</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>18</v>
@@ -38391,16 +38507,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>793</v>
+        <v>799</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>794</v>
+        <v>800</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>795</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>789</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -38439,16 +38555,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>796</v>
+        <v>802</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>797</v>
+        <v>803</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>798</v>
+        <v>804</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>18</v>
@@ -38487,16 +38603,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>799</v>
+        <v>805</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>800</v>
+        <v>806</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>801</v>
+        <v>807</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -38535,16 +38651,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>802</v>
+        <v>808</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>803</v>
+        <v>809</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>804</v>
+        <v>810</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -38553,7 +38669,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="94" t="s">
-        <v>805</v>
+        <v>811</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="9">
@@ -38585,16 +38701,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>806</v>
+        <v>812</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>807</v>
+        <v>813</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>808</v>
+        <v>814</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -38603,7 +38719,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="94" t="s">
-        <v>809</v>
+        <v>815</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="9">
@@ -38646,16 +38762,16 @@
     </row>
     <row r="29">
       <c r="A29" s="65" t="s">
-        <v>810</v>
+        <v>816</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>811</v>
+        <v>817</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>812</v>
+        <v>818</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>34</v>
@@ -38664,7 +38780,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="121" t="s">
-        <v>813</v>
+        <v>819</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="9">
@@ -38694,16 +38810,16 @@
     </row>
     <row r="30">
       <c r="A30" s="123" t="s">
-        <v>814</v>
+        <v>820</v>
       </c>
       <c r="B30" s="124" t="s">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="C30" s="125" t="s">
-        <v>816</v>
+        <v>822</v>
       </c>
       <c r="D30" s="126" t="s">
-        <v>817</v>
+        <v>823</v>
       </c>
       <c r="E30" s="126" t="s">
         <v>18</v>
@@ -38712,7 +38828,7 @@
       <c r="G30" s="127"/>
       <c r="H30" s="127"/>
       <c r="I30" s="121" t="s">
-        <v>818</v>
+        <v>824</v>
       </c>
       <c r="J30" s="128" t="s">
         <v>454</v>
@@ -38750,16 +38866,16 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>819</v>
+        <v>825</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>820</v>
+        <v>826</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>821</v>
+        <v>827</v>
       </c>
       <c r="D31" s="114" t="s">
-        <v>817</v>
+        <v>823</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>18</v>
@@ -38796,16 +38912,16 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>822</v>
+        <v>828</v>
       </c>
       <c r="B32" s="58" t="s">
+        <v>829</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="D32" s="114" t="s">
         <v>823</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>824</v>
-      </c>
-      <c r="D32" s="114" t="s">
-        <v>817</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>18</v>
@@ -43626,19 +43742,19 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>825</v>
+        <v>831</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>826</v>
+        <v>832</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>827</v>
+        <v>833</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>432</v>
@@ -43676,22 +43792,22 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>828</v>
+        <v>834</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>829</v>
+        <v>835</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>830</v>
+        <v>836</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>831</v>
+        <v>837</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -43708,7 +43824,7 @@
         <v>81</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>832</v>
+        <v>838</v>
       </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -43726,22 +43842,22 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>833</v>
+        <v>839</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>834</v>
+        <v>840</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>835</v>
+        <v>841</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>767</v>
+        <v>773</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>831</v>
+        <v>837</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -43758,7 +43874,7 @@
         <v>81</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>832</v>
+        <v>838</v>
       </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -43776,22 +43892,22 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>836</v>
+        <v>842</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>837</v>
+        <v>843</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>838</v>
+        <v>844</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>831</v>
+        <v>837</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -43808,7 +43924,7 @@
         <v>81</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>832</v>
+        <v>838</v>
       </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>

</xml_diff>

<commit_message>
WIP: 002 generated purposes
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/purpose_processing.xlsx
+++ b/documentation-generator/vocab_csv/purpose_processing.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="844">
   <si>
     <t>Term</t>
   </si>
@@ -1498,9 +1498,6 @@
   </si>
   <si>
     <t>ParentProperty</t>
-  </si>
-  <si>
-    <t>CreationDate</t>
   </si>
   <si>
     <t>hasPurpose</t>
@@ -4201,8 +4198,8 @@
       <c r="D9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>34</v>
+      <c r="E9" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -4251,8 +4248,8 @@
       <c r="D10" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>34</v>
+      <c r="E10" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14" t="s">
@@ -4303,8 +4300,8 @@
       <c r="D11" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>34</v>
+      <c r="E11" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
@@ -4355,8 +4352,8 @@
       <c r="D12" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>34</v>
+      <c r="E12" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
@@ -4407,8 +4404,8 @@
       <c r="D13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>34</v>
+      <c r="E13" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -4457,8 +4454,8 @@
       <c r="D14" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>34</v>
+      <c r="E14" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
@@ -4578,8 +4575,8 @@
       <c r="D17" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>34</v>
+      <c r="E17" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
@@ -4628,8 +4625,8 @@
       <c r="D18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>34</v>
+      <c r="E18" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14" t="s">
@@ -4682,8 +4679,8 @@
       <c r="D19" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>34</v>
+      <c r="E19" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11" t="s">
@@ -4734,8 +4731,8 @@
       <c r="D20" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>34</v>
+      <c r="E20" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -4784,8 +4781,8 @@
       <c r="D21" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>34</v>
+      <c r="E21" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -4834,8 +4831,8 @@
       <c r="D22" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>34</v>
+      <c r="E22" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -4884,8 +4881,8 @@
       <c r="D23" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="41" t="s">
-        <v>34</v>
+      <c r="E23" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
@@ -5052,8 +5049,8 @@
       <c r="D27" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>34</v>
+      <c r="E27" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -5102,8 +5099,8 @@
       <c r="D28" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>34</v>
+      <c r="E28" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
@@ -5154,8 +5151,8 @@
       <c r="D29" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>34</v>
+      <c r="E29" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -5204,8 +5201,8 @@
       <c r="D30" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>34</v>
+      <c r="E30" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -5256,8 +5253,8 @@
       <c r="D31" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>34</v>
+      <c r="E31" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -5306,8 +5303,8 @@
       <c r="D32" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>34</v>
+      <c r="E32" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
@@ -5408,8 +5405,8 @@
       <c r="D35" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="E35" s="11" t="s">
-        <v>34</v>
+      <c r="E35" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="34"/>
@@ -5460,8 +5457,8 @@
       <c r="D36" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>34</v>
+      <c r="E36" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="34"/>
@@ -5512,8 +5509,8 @@
       <c r="D37" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="E37" s="11" t="s">
-        <v>34</v>
+      <c r="E37" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="34"/>
@@ -5564,8 +5561,8 @@
       <c r="D38" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="E38" s="11" t="s">
-        <v>34</v>
+      <c r="E38" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="34"/>
@@ -5668,8 +5665,8 @@
       <c r="D40" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>34</v>
+      <c r="E40" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F40" s="34"/>
       <c r="G40" s="34"/>
@@ -5720,8 +5717,8 @@
       <c r="D41" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="E41" s="11" t="s">
-        <v>34</v>
+      <c r="E41" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F41" s="34"/>
       <c r="G41" s="34"/>
@@ -5770,8 +5767,8 @@
       <c r="D42" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>34</v>
+      <c r="E42" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
@@ -5924,8 +5921,8 @@
       <c r="D45" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="E45" s="11" t="s">
-        <v>34</v>
+      <c r="E45" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F45" s="34"/>
       <c r="G45" s="34"/>
@@ -5976,8 +5973,8 @@
       <c r="D46" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>34</v>
+      <c r="E46" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F46" s="34"/>
       <c r="G46" s="34"/>
@@ -6028,8 +6025,8 @@
       <c r="D47" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="E47" s="11" t="s">
-        <v>34</v>
+      <c r="E47" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F47" s="34"/>
       <c r="G47" s="34"/>
@@ -6080,8 +6077,8 @@
       <c r="D48" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>34</v>
+      <c r="E48" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
@@ -6130,8 +6127,8 @@
       <c r="D49" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="E49" s="11" t="s">
-        <v>34</v>
+      <c r="E49" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
@@ -6180,8 +6177,8 @@
       <c r="D50" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>34</v>
+      <c r="E50" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
@@ -6299,8 +6296,8 @@
       <c r="D53" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E53" s="11" t="s">
-        <v>34</v>
+      <c r="E53" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="14"/>
@@ -6350,7 +6347,7 @@
         <v>217</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
@@ -6404,7 +6401,7 @@
         <v>217</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="23" t="s">
@@ -6458,7 +6455,7 @@
         <v>227</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F56" s="23"/>
       <c r="G56" s="23"/>
@@ -6512,7 +6509,7 @@
         <v>227</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="23"/>
@@ -6561,8 +6558,8 @@
       <c r="D58" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="E58" s="11" t="s">
-        <v>34</v>
+      <c r="E58" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F58" s="14"/>
       <c r="G58" s="14"/>
@@ -6680,8 +6677,8 @@
       <c r="D61" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E61" s="11" t="s">
-        <v>34</v>
+      <c r="E61" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F61" s="14"/>
       <c r="G61" s="14" t="s">
@@ -6732,8 +6729,8 @@
       <c r="D62" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E62" s="11" t="s">
-        <v>34</v>
+      <c r="E62" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F62" s="14"/>
       <c r="G62" s="14" t="s">
@@ -6784,8 +6781,8 @@
       <c r="D63" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="E63" s="11" t="s">
-        <v>34</v>
+      <c r="E63" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
@@ -6839,8 +6836,8 @@
       <c r="D66" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E66" s="11" t="s">
-        <v>34</v>
+      <c r="E66" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F66" s="14"/>
       <c r="G66" s="14"/>
@@ -6891,8 +6888,8 @@
       <c r="D67" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E67" s="11" t="s">
-        <v>34</v>
+      <c r="E67" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F67" s="14"/>
       <c r="G67" s="14"/>
@@ -6943,8 +6940,8 @@
       <c r="D68" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E68" s="11" t="s">
-        <v>34</v>
+      <c r="E68" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
@@ -6995,8 +6992,8 @@
       <c r="D69" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="E69" s="11" t="s">
-        <v>34</v>
+      <c r="E69" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F69" s="14"/>
       <c r="G69" s="14"/>
@@ -7114,8 +7111,8 @@
       <c r="D72" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="E72" s="66" t="s">
-        <v>34</v>
+      <c r="E72" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F72" s="26"/>
       <c r="G72" s="26"/>
@@ -7164,8 +7161,8 @@
       <c r="D73" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="E73" s="11" t="s">
-        <v>34</v>
+      <c r="E73" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F73" s="14"/>
       <c r="G73" s="14"/>
@@ -7215,7 +7212,7 @@
         <v>266</v>
       </c>
       <c r="E74" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F74" s="23"/>
       <c r="G74" s="23"/>
@@ -7266,8 +7263,8 @@
       <c r="D75" s="72" t="s">
         <v>266</v>
       </c>
-      <c r="E75" s="11" t="s">
-        <v>34</v>
+      <c r="E75" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F75" s="14"/>
       <c r="G75" s="14"/>
@@ -7318,8 +7315,8 @@
       <c r="D76" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="E76" s="11" t="s">
-        <v>34</v>
+      <c r="E76" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F76" s="14"/>
       <c r="G76" s="14"/>
@@ -7366,8 +7363,8 @@
       <c r="D77" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="E77" s="11" t="s">
-        <v>34</v>
+      <c r="E77" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F77" s="14"/>
       <c r="G77" s="14"/>
@@ -7420,8 +7417,8 @@
       <c r="D78" s="72" t="s">
         <v>266</v>
       </c>
-      <c r="E78" s="11" t="s">
-        <v>34</v>
+      <c r="E78" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F78" s="14"/>
       <c r="G78" s="14"/>
@@ -7470,8 +7467,8 @@
       <c r="D79" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="E79" s="11" t="s">
-        <v>34</v>
+      <c r="E79" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F79" s="14"/>
       <c r="G79" s="14" t="s">
@@ -7522,8 +7519,8 @@
       <c r="D80" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="E80" s="5" t="s">
-        <v>34</v>
+      <c r="E80" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
@@ -7573,8 +7570,8 @@
       <c r="D82" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="E82" s="11" t="s">
-        <v>34</v>
+      <c r="E82" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F82" s="14"/>
       <c r="G82" s="14"/>
@@ -7626,7 +7623,7 @@
         <v>314</v>
       </c>
       <c r="E83" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F83" s="23"/>
       <c r="G83" s="23" t="s">
@@ -7679,8 +7676,8 @@
       <c r="D84" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="E84" s="11" t="s">
-        <v>34</v>
+      <c r="E84" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F84" s="14"/>
       <c r="G84" s="14"/>
@@ -7729,8 +7726,8 @@
       <c r="D85" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="E85" s="11" t="s">
-        <v>34</v>
+      <c r="E85" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F85" s="14"/>
       <c r="G85" s="14"/>
@@ -7779,8 +7776,8 @@
       <c r="D86" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="E86" s="11" t="s">
-        <v>34</v>
+      <c r="E86" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
@@ -7829,8 +7826,8 @@
       <c r="D87" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="E87" s="11" t="s">
-        <v>34</v>
+      <c r="E87" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F87" s="14"/>
       <c r="G87" s="14"/>
@@ -7879,8 +7876,8 @@
       <c r="D88" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="E88" s="11" t="s">
-        <v>34</v>
+      <c r="E88" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F88" s="14"/>
       <c r="G88" s="14"/>
@@ -7929,8 +7926,8 @@
       <c r="D89" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="E89" s="11" t="s">
-        <v>34</v>
+      <c r="E89" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F89" s="14"/>
       <c r="G89" s="14"/>
@@ -8028,7 +8025,7 @@
         <v>345</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F92" s="23"/>
       <c r="G92" s="23"/>
@@ -8081,8 +8078,8 @@
       <c r="D93" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="E93" s="5" t="s">
-        <v>34</v>
+      <c r="E93" s="21" t="s">
+        <v>33</v>
       </c>
       <c r="F93" s="8"/>
       <c r="G93" s="8"/>
@@ -8501,7 +8498,9 @@
       <c r="D105" s="78" t="s">
         <v>241</v>
       </c>
-      <c r="E105" s="37"/>
+      <c r="E105" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="F105" s="37"/>
       <c r="G105" s="78"/>
       <c r="H105" s="37"/>
@@ -11700,7 +11699,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="86" t="s">
-        <v>428</v>
+        <v>10</v>
       </c>
       <c r="L1" s="87" t="s">
         <v>11</v>
@@ -11717,13 +11716,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>430</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>431</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
@@ -11733,7 +11732,7 @@
         <v>dpv:Purpose</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -11751,7 +11750,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>24</v>
@@ -11772,22 +11771,22 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="B3" s="76" t="s">
         <v>434</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="C3" s="5" t="s">
         <v>435</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>436</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -14859,13 +14858,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>438</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>438</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>439</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
@@ -14875,7 +14874,7 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>20</v>
@@ -14929,7 +14928,7 @@
     </row>
     <row r="4">
       <c r="A4" s="65" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -14945,30 +14944,30 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>441</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="B5" s="58" t="s">
-        <v>442</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>444</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="91"/>
       <c r="J5" s="93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -14976,7 +14975,7 @@
         <v>106</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="8"/>
@@ -14997,30 +14996,30 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>448</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>448</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>449</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="91"/>
       <c r="J6" s="93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K6" s="9">
         <v>43592.0</v>
@@ -15031,7 +15030,7 @@
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
@@ -15051,16 +15050,16 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>452</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>453</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>34</v>
@@ -15070,7 +15069,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="91"/>
       <c r="J7" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K7" s="9">
         <v>43592.0</v>
@@ -15081,7 +15080,7 @@
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
@@ -15101,16 +15100,16 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>456</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>34</v>
@@ -15120,7 +15119,7 @@
       <c r="H8" s="8"/>
       <c r="I8" s="91"/>
       <c r="J8" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K8" s="9">
         <v>43592.0</v>
@@ -15131,7 +15130,7 @@
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
@@ -15151,16 +15150,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>457</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>458</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>34</v>
@@ -15170,7 +15169,7 @@
       <c r="H9" s="8"/>
       <c r="I9" s="91"/>
       <c r="J9" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K9" s="9">
         <v>43592.0</v>
@@ -15181,7 +15180,7 @@
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
@@ -15201,16 +15200,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>459</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>460</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>34</v>
@@ -15220,7 +15219,7 @@
       <c r="H10" s="8"/>
       <c r="I10" s="91"/>
       <c r="J10" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K10" s="9">
         <v>43592.0</v>
@@ -15231,7 +15230,7 @@
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
@@ -15251,16 +15250,16 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>460</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="B11" s="76" t="s">
-        <v>461</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>462</v>
-      </c>
       <c r="D11" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>34</v>
@@ -15270,7 +15269,7 @@
       <c r="H11" s="8"/>
       <c r="I11" s="91"/>
       <c r="J11" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K11" s="9">
         <v>43592.0</v>
@@ -15281,7 +15280,7 @@
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
@@ -15301,30 +15300,30 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>462</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="B12" s="76" t="s">
-        <v>463</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>464</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I12" s="91"/>
       <c r="J12" s="93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K12" s="9">
         <v>43592.0</v>
@@ -15335,7 +15334,7 @@
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
@@ -15355,16 +15354,16 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>465</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="B13" s="76" t="s">
-        <v>466</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>467</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>34</v>
@@ -15374,7 +15373,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="91"/>
       <c r="J13" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K13" s="9">
         <v>43592.0</v>
@@ -15385,7 +15384,7 @@
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
@@ -15405,16 +15404,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>469</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>34</v>
@@ -15424,7 +15423,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="91"/>
       <c r="J14" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K14" s="9">
         <v>43592.0</v>
@@ -15435,7 +15434,7 @@
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
@@ -15455,21 +15454,21 @@
     </row>
     <row r="16">
       <c r="A16" s="65" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>471</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>472</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>34</v>
@@ -15510,30 +15509,30 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>473</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>474</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="91"/>
       <c r="J18" s="93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K18" s="9">
         <v>43592.0</v>
@@ -15544,7 +15543,7 @@
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
@@ -15564,16 +15563,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>477</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>34</v>
@@ -15614,30 +15613,30 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>479</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I20" s="91"/>
       <c r="J20" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K20" s="9">
         <v>43592.0</v>
@@ -15648,7 +15647,7 @@
       </c>
       <c r="N20" s="8"/>
       <c r="O20" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
@@ -15668,16 +15667,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>483</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>484</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>34</v>
@@ -15718,16 +15717,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>486</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>34</v>
@@ -15768,16 +15767,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>486</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="B23" s="58" t="s">
-        <v>487</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>488</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>34</v>
@@ -15787,7 +15786,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="91"/>
       <c r="J23" s="93" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K23" s="9">
         <v>44671.0</v>
@@ -15820,16 +15819,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>491</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>34</v>
@@ -15839,7 +15838,7 @@
       <c r="H24" s="8"/>
       <c r="I24" s="91"/>
       <c r="J24" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K24" s="9">
         <v>43592.0</v>
@@ -15850,7 +15849,7 @@
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
@@ -15870,16 +15869,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>493</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>34</v>
@@ -15889,7 +15888,7 @@
       <c r="H25" s="8"/>
       <c r="I25" s="91"/>
       <c r="J25" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K25" s="9">
         <v>43592.0</v>
@@ -15900,7 +15899,7 @@
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
@@ -15920,32 +15919,32 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="M26" s="5" t="s">
         <v>494</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="65" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>499</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>34</v>
@@ -15955,7 +15954,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="91"/>
       <c r="J29" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K29" s="9">
         <v>43592.0</v>
@@ -15966,7 +15965,7 @@
       </c>
       <c r="N29" s="8"/>
       <c r="O29" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
@@ -15986,30 +15985,30 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>501</v>
-      </c>
       <c r="D30" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I30" s="91"/>
       <c r="J30" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K30" s="9">
         <v>43592.0</v>
@@ -16020,7 +16019,7 @@
       </c>
       <c r="N30" s="8"/>
       <c r="O30" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
@@ -16040,32 +16039,32 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>503</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>504</v>
-      </c>
       <c r="D31" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I31" s="94" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J31" s="93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K31" s="9">
         <v>43592.0</v>
@@ -16076,7 +16075,7 @@
       </c>
       <c r="N31" s="8"/>
       <c r="O31" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P31" s="8"/>
       <c r="Q31" s="8"/>
@@ -16096,16 +16095,16 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>506</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="B32" s="58" t="s">
-        <v>507</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>508</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>509</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>34</v>
@@ -16114,7 +16113,7 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="94" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J32" s="92"/>
       <c r="K32" s="9">
@@ -16148,16 +16147,16 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="B33" s="58" t="s">
+        <v>510</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>511</v>
       </c>
-      <c r="B33" s="58" t="s">
-        <v>511</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>512</v>
-      </c>
       <c r="D33" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>34</v>
@@ -16198,16 +16197,16 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>514</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>34</v>
@@ -16248,16 +16247,16 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>515</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>516</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>34</v>
@@ -16267,7 +16266,7 @@
       <c r="H35" s="8"/>
       <c r="I35" s="91"/>
       <c r="J35" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K35" s="9">
         <v>43592.0</v>
@@ -16278,7 +16277,7 @@
       </c>
       <c r="N35" s="8"/>
       <c r="O35" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P35" s="8"/>
       <c r="Q35" s="8"/>
@@ -16311,7 +16310,7 @@
     </row>
     <row r="37">
       <c r="A37" s="65" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -16326,16 +16325,16 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>518</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>519</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>520</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>34</v>
@@ -16345,7 +16344,7 @@
       <c r="H38" s="8"/>
       <c r="I38" s="91"/>
       <c r="J38" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K38" s="9">
         <v>43592.0</v>
@@ -16356,7 +16355,7 @@
       </c>
       <c r="N38" s="8"/>
       <c r="O38" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P38" s="8"/>
       <c r="Q38" s="8"/>
@@ -16376,16 +16375,16 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>521</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>522</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>34</v>
@@ -16395,7 +16394,7 @@
       <c r="H39" s="8"/>
       <c r="I39" s="91"/>
       <c r="J39" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K39" s="9">
         <v>43592.0</v>
@@ -16406,7 +16405,7 @@
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P39" s="8"/>
       <c r="Q39" s="8"/>
@@ -16440,7 +16439,7 @@
     </row>
     <row r="41">
       <c r="A41" s="65" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="5"/>
@@ -16456,30 +16455,30 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>523</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>524</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>525</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I42" s="91"/>
       <c r="J42" s="93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K42" s="9">
         <v>43592.0</v>
@@ -16490,7 +16489,7 @@
       </c>
       <c r="N42" s="8"/>
       <c r="O42" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P42" s="8"/>
       <c r="Q42" s="8"/>
@@ -16523,7 +16522,7 @@
     </row>
     <row r="44">
       <c r="A44" s="65" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -16538,16 +16537,16 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>528</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>529</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>530</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>34</v>
@@ -16557,7 +16556,7 @@
       <c r="H45" s="8"/>
       <c r="I45" s="91"/>
       <c r="J45" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K45" s="9">
         <v>43592.0</v>
@@ -16568,7 +16567,7 @@
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P45" s="8"/>
       <c r="Q45" s="8"/>
@@ -16588,16 +16587,16 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>531</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>531</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>532</v>
-      </c>
       <c r="D46" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>34</v>
@@ -16607,7 +16606,7 @@
       <c r="H46" s="8"/>
       <c r="I46" s="91"/>
       <c r="J46" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K46" s="9">
         <v>43592.0</v>
@@ -16618,7 +16617,7 @@
       </c>
       <c r="N46" s="8"/>
       <c r="O46" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P46" s="8"/>
       <c r="Q46" s="8"/>
@@ -16638,16 +16637,16 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>534</v>
-      </c>
       <c r="D47" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>34</v>
@@ -16657,7 +16656,7 @@
       <c r="H47" s="8"/>
       <c r="I47" s="91"/>
       <c r="J47" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K47" s="9">
         <v>43592.0</v>
@@ -16668,7 +16667,7 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P47" s="8"/>
       <c r="Q47" s="8"/>
@@ -16688,16 +16687,16 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>535</v>
-      </c>
-      <c r="C48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>536</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>537</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>34</v>
@@ -16738,30 +16737,30 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>538</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>538</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>539</v>
-      </c>
       <c r="D49" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I49" s="91"/>
       <c r="J49" s="93" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K49" s="9">
         <v>43592.0</v>
@@ -16772,7 +16771,7 @@
       </c>
       <c r="N49" s="8"/>
       <c r="O49" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P49" s="8"/>
       <c r="Q49" s="8"/>
@@ -16792,30 +16791,30 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>541</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>542</v>
-      </c>
       <c r="D50" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>20</v>
       </c>
       <c r="I50" s="91"/>
       <c r="J50" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K50" s="9">
         <v>43592.0</v>
@@ -16826,7 +16825,7 @@
       </c>
       <c r="N50" s="8"/>
       <c r="O50" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P50" s="8"/>
       <c r="Q50" s="8"/>
@@ -16846,16 +16845,16 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>543</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>543</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>544</v>
-      </c>
       <c r="D51" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>34</v>
@@ -16896,16 +16895,16 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="B52" s="58" t="s">
+        <v>544</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>545</v>
       </c>
-      <c r="B52" s="58" t="s">
-        <v>545</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>546</v>
-      </c>
       <c r="D52" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>34</v>
@@ -16915,7 +16914,7 @@
       <c r="H52" s="8"/>
       <c r="I52" s="91"/>
       <c r="J52" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K52" s="9">
         <v>43592.0</v>
@@ -16928,7 +16927,7 @@
         <v>44848.0</v>
       </c>
       <c r="O52" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P52" s="8"/>
       <c r="Q52" s="8"/>
@@ -16946,16 +16945,16 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="C53" s="95" t="s">
         <v>547</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>547</v>
-      </c>
-      <c r="C53" s="95" t="s">
-        <v>548</v>
-      </c>
       <c r="D53" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>34</v>
@@ -16965,7 +16964,7 @@
       <c r="H53" s="8"/>
       <c r="I53" s="91"/>
       <c r="J53" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K53" s="9">
         <v>43592.0</v>
@@ -16976,7 +16975,7 @@
       </c>
       <c r="N53" s="8"/>
       <c r="O53" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P53" s="8"/>
       <c r="Q53" s="8"/>
@@ -16996,16 +16995,16 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>549</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>550</v>
-      </c>
       <c r="D54" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>34</v>
@@ -17046,19 +17045,19 @@
     </row>
     <row r="56">
       <c r="A56" s="65" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B57" s="58"/>
       <c r="C57" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="D57" s="38" t="s">
         <v>553</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>554</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>34</v>
@@ -17068,7 +17067,7 @@
       <c r="H57" s="8"/>
       <c r="I57" s="91"/>
       <c r="J57" s="96" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
@@ -17095,14 +17094,14 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B58" s="58"/>
       <c r="C58" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>34</v>
@@ -17112,7 +17111,7 @@
       <c r="H58" s="8"/>
       <c r="I58" s="91"/>
       <c r="J58" s="96" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
@@ -17139,16 +17138,16 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="B59" s="58" t="s">
+        <v>558</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="B59" s="58" t="s">
-        <v>559</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>560</v>
-      </c>
       <c r="D59" s="38" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>34</v>
@@ -17158,7 +17157,7 @@
       <c r="H59" s="8"/>
       <c r="I59" s="91"/>
       <c r="J59" s="96" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
@@ -17166,7 +17165,7 @@
         <v>106</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="O59" s="5"/>
       <c r="P59" s="8"/>
@@ -17187,16 +17186,16 @@
     </row>
     <row r="60">
       <c r="A60" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="C60" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>563</v>
-      </c>
       <c r="D60" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>34</v>
@@ -17206,7 +17205,7 @@
       <c r="H60" s="8"/>
       <c r="I60" s="91"/>
       <c r="J60" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K60" s="9">
         <v>43592.0</v>
@@ -17217,7 +17216,7 @@
       </c>
       <c r="N60" s="8"/>
       <c r="O60" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P60" s="8"/>
       <c r="Q60" s="8"/>
@@ -17237,16 +17236,16 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>564</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>564</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>565</v>
-      </c>
       <c r="D61" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>34</v>
@@ -17256,7 +17255,7 @@
       <c r="H61" s="8"/>
       <c r="I61" s="91"/>
       <c r="J61" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K61" s="9">
         <v>43592.0</v>
@@ -17267,7 +17266,7 @@
       </c>
       <c r="N61" s="8"/>
       <c r="O61" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P61" s="8"/>
       <c r="Q61" s="8"/>
@@ -17287,16 +17286,16 @@
     </row>
     <row r="62">
       <c r="A62" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>566</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C62" s="7" t="s">
         <v>567</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>568</v>
-      </c>
       <c r="D62" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>34</v>
@@ -17306,7 +17305,7 @@
       <c r="H62" s="8"/>
       <c r="I62" s="91"/>
       <c r="J62" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K62" s="9">
         <v>43592.0</v>
@@ -17317,7 +17316,7 @@
       </c>
       <c r="N62" s="8"/>
       <c r="O62" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P62" s="8"/>
       <c r="Q62" s="8"/>
@@ -17337,16 +17336,16 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="B63" s="76" t="s">
+        <v>568</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>569</v>
       </c>
-      <c r="B63" s="76" t="s">
-        <v>569</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>570</v>
-      </c>
       <c r="D63" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>34</v>
@@ -17356,7 +17355,7 @@
       <c r="H63" s="8"/>
       <c r="I63" s="91"/>
       <c r="J63" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K63" s="9">
         <v>43592.0</v>
@@ -17367,7 +17366,7 @@
       </c>
       <c r="N63" s="8"/>
       <c r="O63" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P63" s="8"/>
       <c r="Q63" s="8"/>
@@ -17387,16 +17386,16 @@
     </row>
     <row r="64">
       <c r="A64" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="B64" s="76" t="s">
+        <v>570</v>
+      </c>
+      <c r="C64" s="7" t="s">
         <v>571</v>
       </c>
-      <c r="B64" s="76" t="s">
-        <v>571</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>572</v>
-      </c>
       <c r="D64" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>34</v>
@@ -17406,7 +17405,7 @@
       <c r="H64" s="8"/>
       <c r="I64" s="91"/>
       <c r="J64" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K64" s="9">
         <v>43592.0</v>
@@ -17417,7 +17416,7 @@
       </c>
       <c r="N64" s="8"/>
       <c r="O64" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P64" s="8"/>
       <c r="Q64" s="8"/>
@@ -17437,21 +17436,21 @@
     </row>
     <row r="66">
       <c r="A66" s="65" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B67" s="76" t="s">
+        <v>573</v>
+      </c>
+      <c r="C67" s="7" t="s">
         <v>574</v>
       </c>
-      <c r="B67" s="76" t="s">
-        <v>574</v>
-      </c>
-      <c r="C67" s="7" t="s">
+      <c r="D67" s="5" t="s">
         <v>575</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>576</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>34</v>
@@ -17461,7 +17460,7 @@
       <c r="H67" s="8"/>
       <c r="I67" s="91"/>
       <c r="J67" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K67" s="9">
         <v>43592.0</v>
@@ -17472,7 +17471,7 @@
       </c>
       <c r="N67" s="8"/>
       <c r="O67" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P67" s="8"/>
       <c r="Q67" s="8"/>
@@ -17492,16 +17491,16 @@
     </row>
     <row r="68">
       <c r="A68" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="B68" s="58" t="s">
+        <v>576</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>577</v>
       </c>
-      <c r="B68" s="58" t="s">
-        <v>577</v>
-      </c>
-      <c r="C68" s="7" t="s">
+      <c r="D68" s="5" t="s">
         <v>578</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>579</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>34</v>
@@ -17538,16 +17537,16 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="B69" s="58" t="s">
+        <v>579</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="B69" s="58" t="s">
-        <v>580</v>
-      </c>
-      <c r="C69" s="7" t="s">
+      <c r="D69" s="5" t="s">
         <v>581</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>582</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>34</v>
@@ -22482,13 +22481,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>582</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>584</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>585</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
@@ -22498,7 +22497,7 @@
         <v>dpv:Processing</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -22516,7 +22515,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>24</v>
@@ -26554,22 +26553,22 @@
     </row>
     <row r="2">
       <c r="A2" s="101" t="s">
+        <v>585</v>
+      </c>
+      <c r="B2" s="101" t="s">
         <v>586</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="C2" s="102" t="s">
         <v>587</v>
-      </c>
-      <c r="C2" s="102" t="s">
-        <v>588</v>
       </c>
       <c r="D2" s="101" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="101" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19"/>
@@ -26583,7 +26582,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="101" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O2" s="105" t="s">
         <v>51</v>
@@ -26604,38 +26603,38 @@
     </row>
     <row r="3">
       <c r="A3" s="106" t="s">
+        <v>590</v>
+      </c>
+      <c r="B3" s="107" t="s">
         <v>591</v>
       </c>
-      <c r="B3" s="107" t="s">
+      <c r="C3" s="106" t="s">
         <v>592</v>
-      </c>
-      <c r="C3" s="106" t="s">
-        <v>593</v>
       </c>
       <c r="D3" s="106" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="106" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G3" s="108"/>
       <c r="H3" s="108"/>
       <c r="I3" s="108"/>
       <c r="J3" s="109" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="K3" s="104">
         <v>44786.0</v>
       </c>
       <c r="L3" s="110"/>
       <c r="M3" s="101" t="s">
+        <v>595</v>
+      </c>
+      <c r="N3" s="101" t="s">
         <v>596</v>
-      </c>
-      <c r="N3" s="101" t="s">
-        <v>597</v>
       </c>
       <c r="O3" s="111" t="s">
         <v>24</v>
@@ -26656,22 +26655,22 @@
     </row>
     <row r="4">
       <c r="A4" s="113" t="s">
+        <v>597</v>
+      </c>
+      <c r="B4" s="113" t="s">
         <v>598</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="C4" s="101" t="s">
         <v>599</v>
-      </c>
-      <c r="C4" s="101" t="s">
-        <v>600</v>
       </c>
       <c r="D4" s="101" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="101" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G4" s="102"/>
       <c r="H4" s="102"/>
@@ -26684,10 +26683,10 @@
         <v>44727.0</v>
       </c>
       <c r="M4" s="101" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="N4" s="101" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O4" s="105" t="s">
         <v>99</v>
@@ -26708,22 +26707,22 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>601</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>603</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>604</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -26756,27 +26755,27 @@
     </row>
     <row r="6">
       <c r="A6" s="113" t="s">
+        <v>605</v>
+      </c>
+      <c r="B6" s="113" t="s">
         <v>606</v>
       </c>
-      <c r="B6" s="113" t="s">
+      <c r="C6" s="101" t="s">
         <v>607</v>
-      </c>
-      <c r="C6" s="101" t="s">
-        <v>608</v>
       </c>
       <c r="D6" s="101" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G6" s="102"/>
       <c r="H6" s="102"/>
       <c r="I6" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="104">
@@ -26787,7 +26786,7 @@
         <v>22</v>
       </c>
       <c r="N6" s="101" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O6" s="105" t="s">
         <v>51</v>
@@ -30948,16 +30947,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="B2" s="58" t="s">
         <v>611</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="C2" s="7" t="s">
         <v>612</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>613</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>614</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>34</v>
@@ -31009,7 +31008,7 @@
     </row>
     <row r="4">
       <c r="A4" s="65" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B4" s="58"/>
       <c r="C4" s="7"/>
@@ -31024,16 +31023,16 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="B5" s="58" t="s">
         <v>616</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="C5" s="7" t="s">
         <v>617</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>618</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>34</v>
@@ -31042,7 +31041,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="94" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="9">
@@ -31078,16 +31077,16 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="B6" s="58" t="s">
         <v>620</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="C6" s="7" t="s">
         <v>621</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>622</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>623</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>34</v>
@@ -31126,16 +31125,16 @@
     </row>
     <row r="7">
       <c r="A7" s="114" t="s">
+        <v>623</v>
+      </c>
+      <c r="B7" s="115" t="s">
         <v>624</v>
       </c>
-      <c r="B7" s="115" t="s">
+      <c r="C7" s="7" t="s">
         <v>625</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>626</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>627</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>34</v>
@@ -31144,10 +31143,10 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J7" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K7" s="9">
         <v>44139.0</v>
@@ -31159,7 +31158,7 @@
         <v>294</v>
       </c>
       <c r="N7" s="114" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>99</v>
@@ -31193,16 +31192,16 @@
     </row>
     <row r="9">
       <c r="A9" s="65" t="s">
+        <v>629</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>630</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>631</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>632</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>34</v>
@@ -31211,7 +31210,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="94" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="9">
@@ -31245,16 +31244,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>634</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="7" t="s">
         <v>635</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>636</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>637</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
@@ -31263,7 +31262,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="94" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="9">
@@ -31299,16 +31298,16 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="7" t="s">
         <v>640</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>641</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>642</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>18</v>
@@ -31317,7 +31316,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="94" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="9">
@@ -31353,16 +31352,16 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>644</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="7" t="s">
         <v>645</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>646</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>647</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>18</v>
@@ -31371,7 +31370,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="94" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="9">
@@ -31405,16 +31404,16 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="7" t="s">
         <v>650</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>651</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
@@ -31423,7 +31422,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="94" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="9">
@@ -31457,16 +31456,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>655</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>18</v>
@@ -31507,16 +31506,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>656</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>658</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>18</v>
@@ -31525,7 +31524,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="94" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="9">
@@ -31572,16 +31571,16 @@
     </row>
     <row r="17">
       <c r="A17" s="65" t="s">
+        <v>659</v>
+      </c>
+      <c r="B17" s="58" t="s">
         <v>660</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="C17" s="7" t="s">
         <v>661</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>662</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>34</v>
@@ -31590,7 +31589,7 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="94" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="9">
@@ -31626,16 +31625,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>666</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
@@ -31674,16 +31673,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>667</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="7" t="s">
         <v>668</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>669</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>18</v>
@@ -31722,16 +31721,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>672</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>18</v>
@@ -31784,7 +31783,7 @@
     </row>
     <row r="22">
       <c r="A22" s="65" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B22" s="58"/>
       <c r="C22" s="7"/>
@@ -31800,16 +31799,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="B23" s="58" t="s">
         <v>674</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="C23" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>676</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -31818,7 +31817,7 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="94" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J23" s="92"/>
       <c r="K23" s="9">
@@ -31829,7 +31828,7 @@
         <v>22</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="O23" s="114"/>
       <c r="P23" s="8"/>
@@ -31850,16 +31849,16 @@
     </row>
     <row r="24">
       <c r="A24" s="114" t="s">
+        <v>678</v>
+      </c>
+      <c r="B24" s="115" t="s">
+        <v>672</v>
+      </c>
+      <c r="C24" s="117" t="s">
         <v>679</v>
       </c>
-      <c r="B24" s="115" t="s">
-        <v>673</v>
-      </c>
-      <c r="C24" s="117" t="s">
-        <v>680</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>34</v>
@@ -31868,7 +31867,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="118" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J24" s="114"/>
       <c r="K24" s="9">
@@ -31902,16 +31901,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="B25" s="58" t="s">
         <v>682</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="C25" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>684</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -31929,7 +31928,7 @@
         <v>22</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="O25" s="114"/>
       <c r="P25" s="8"/>
@@ -31950,16 +31949,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="B26" s="58" t="s">
         <v>686</v>
       </c>
-      <c r="B26" s="58" t="s">
+      <c r="C26" s="7" t="s">
         <v>687</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>688</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -31968,7 +31967,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="94" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="J26" s="114"/>
       <c r="K26" s="9">
@@ -31979,7 +31978,7 @@
         <v>22</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="O26" s="114"/>
       <c r="P26" s="8"/>
@@ -32000,13 +31999,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>689</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>690</v>
-      </c>
-      <c r="B27" s="58" t="s">
-        <v>690</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>691</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -32040,13 +32039,13 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="B28" s="58" t="s">
+        <v>691</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>692</v>
-      </c>
-      <c r="B28" s="58" t="s">
-        <v>692</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>693</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -32080,13 +32079,13 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>693</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>694</v>
-      </c>
-      <c r="B29" s="58" t="s">
-        <v>694</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>695</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -32134,7 +32133,7 @@
     </row>
     <row r="31">
       <c r="A31" s="65" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B31" s="115"/>
       <c r="C31" s="7"/>
@@ -32150,16 +32149,16 @@
     </row>
     <row r="32">
       <c r="A32" s="114" t="s">
+        <v>696</v>
+      </c>
+      <c r="B32" s="115" t="s">
         <v>697</v>
       </c>
-      <c r="B32" s="115" t="s">
+      <c r="C32" s="7" t="s">
         <v>698</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>699</v>
-      </c>
       <c r="D32" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>34</v>
@@ -32169,7 +32168,7 @@
       <c r="H32" s="8"/>
       <c r="I32" s="91"/>
       <c r="J32" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K32" s="9">
         <v>44139.0</v>
@@ -32179,7 +32178,7 @@
         <v>22</v>
       </c>
       <c r="N32" s="114" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O32" s="114" t="s">
         <v>51</v>
@@ -32202,16 +32201,16 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="7" t="s">
         <v>701</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>702</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>703</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>34</v>
@@ -32221,7 +32220,7 @@
       <c r="H33" s="8"/>
       <c r="I33" s="91"/>
       <c r="J33" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K33" s="9">
         <v>44856.0</v>
@@ -32252,16 +32251,16 @@
     </row>
     <row r="34">
       <c r="A34" s="5" t="s">
+        <v>703</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>704</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="7" t="s">
         <v>705</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>706</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>34</v>
@@ -32271,7 +32270,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="91"/>
       <c r="J34" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K34" s="9">
         <v>44856.0</v>
@@ -32302,16 +32301,16 @@
     </row>
     <row r="35">
       <c r="A35" s="114" t="s">
+        <v>706</v>
+      </c>
+      <c r="B35" s="115" t="s">
         <v>707</v>
       </c>
-      <c r="B35" s="115" t="s">
+      <c r="C35" s="7" t="s">
         <v>708</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>709</v>
-      </c>
       <c r="D35" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -32319,7 +32318,7 @@
       <c r="H35" s="8"/>
       <c r="I35" s="91"/>
       <c r="J35" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K35" s="9">
         <v>44139.0</v>
@@ -32329,7 +32328,7 @@
         <v>289</v>
       </c>
       <c r="N35" s="114" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O35" s="40" t="s">
         <v>82</v>
@@ -32350,16 +32349,16 @@
     </row>
     <row r="37">
       <c r="A37" s="114" t="s">
+        <v>709</v>
+      </c>
+      <c r="B37" s="115" t="s">
         <v>710</v>
       </c>
-      <c r="B37" s="115" t="s">
+      <c r="C37" s="117" t="s">
         <v>711</v>
       </c>
-      <c r="C37" s="117" t="s">
-        <v>712</v>
-      </c>
       <c r="D37" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>34</v>
@@ -32369,7 +32368,7 @@
       <c r="H37" s="8"/>
       <c r="I37" s="91"/>
       <c r="J37" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K37" s="9">
         <v>44139.0</v>
@@ -32379,7 +32378,7 @@
         <v>22</v>
       </c>
       <c r="N37" s="114" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O37" s="114" t="s">
         <v>51</v>
@@ -32402,16 +32401,16 @@
     </row>
     <row r="39">
       <c r="A39" s="65" t="s">
+        <v>712</v>
+      </c>
+      <c r="B39" s="58" t="s">
         <v>713</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="C39" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>715</v>
-      </c>
       <c r="D39" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>34</v>
@@ -32429,7 +32428,7 @@
         <v>22</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="O39" s="120" t="s">
         <v>24</v>
@@ -32452,16 +32451,16 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
+        <v>715</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>716</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>717</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>718</v>
-      </c>
       <c r="D40" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>34</v>
@@ -32479,7 +32478,7 @@
         <v>22</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="O40" s="120" t="s">
         <v>24</v>
@@ -32502,16 +32501,16 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>721</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>722</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>34</v>
@@ -32529,7 +32528,7 @@
         <v>22</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="O41" s="120" t="s">
         <v>24</v>
@@ -32552,16 +32551,16 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
+        <v>722</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>723</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>724</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>725</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>726</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>34</v>
@@ -32579,7 +32578,7 @@
         <v>22</v>
       </c>
       <c r="N42" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="O42" s="120" t="s">
         <v>24</v>
@@ -32602,16 +32601,16 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>727</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>728</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>729</v>
-      </c>
       <c r="D43" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>34</v>
@@ -32629,7 +32628,7 @@
         <v>22</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="O43" s="120" t="s">
         <v>24</v>
@@ -32652,16 +32651,16 @@
     </row>
     <row r="44">
       <c r="A44" s="114" t="s">
+        <v>729</v>
+      </c>
+      <c r="B44" s="115" t="s">
         <v>730</v>
       </c>
-      <c r="B44" s="115" t="s">
+      <c r="C44" s="117" t="s">
         <v>731</v>
       </c>
-      <c r="C44" s="117" t="s">
-        <v>732</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>34</v>
@@ -32671,7 +32670,7 @@
       <c r="H44" s="8"/>
       <c r="I44" s="91"/>
       <c r="J44" s="93" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K44" s="9">
         <v>44139.0</v>
@@ -32681,7 +32680,7 @@
         <v>22</v>
       </c>
       <c r="N44" s="114" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O44" s="114" t="s">
         <v>51</v>
@@ -32709,10 +32708,10 @@
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>733</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>734</v>
       </c>
       <c r="C46" s="98"/>
       <c r="D46" s="8"/>
@@ -32747,10 +32746,10 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>735</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>736</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
@@ -32785,10 +32784,10 @@
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>737</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>738</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="8"/>
@@ -37605,16 +37604,16 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>738</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>739</v>
       </c>
-      <c r="B2" s="58" t="s">
-        <v>739</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>740</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>34</v>
@@ -37623,7 +37622,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="94" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="9">
@@ -37634,7 +37633,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>99</v>
@@ -37667,16 +37666,16 @@
     </row>
     <row r="4">
       <c r="A4" s="65" t="s">
+        <v>742</v>
+      </c>
+      <c r="B4" s="58" t="s">
         <v>743</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="C4" s="7" t="s">
         <v>744</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>745</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>746</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>34</v>
@@ -37694,7 +37693,7 @@
         <v>22</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="O4" s="10" t="s">
         <v>99</v>
@@ -37715,16 +37714,16 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="B5" s="58" t="s">
         <v>747</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="C5" s="7" t="s">
         <v>748</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>749</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>750</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>18</v>
@@ -37763,16 +37762,16 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="B6" s="58" t="s">
         <v>751</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="C6" s="7" t="s">
         <v>752</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>753</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>18</v>
@@ -37811,16 +37810,16 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="B7" s="58" t="s">
         <v>754</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="C7" s="7" t="s">
         <v>755</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>756</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>18</v>
@@ -37838,7 +37837,7 @@
         <v>22</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="O7" s="10" t="s">
         <v>99</v>
@@ -37859,16 +37858,16 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B8" s="58" t="s">
         <v>758</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="C8" s="7" t="s">
         <v>759</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>760</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>18</v>
@@ -37907,16 +37906,16 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="B9" s="58" t="s">
         <v>761</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="C9" s="99" t="s">
         <v>762</v>
       </c>
-      <c r="C9" s="99" t="s">
-        <v>763</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>18</v>
@@ -37955,16 +37954,16 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="B10" s="58" t="s">
         <v>764</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="C10" s="7" t="s">
         <v>765</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>766</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>18</v>
@@ -38015,16 +38014,16 @@
     </row>
     <row r="12">
       <c r="A12" s="65" t="s">
+        <v>766</v>
+      </c>
+      <c r="B12" s="58" t="s">
         <v>767</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="C12" s="7" t="s">
         <v>768</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>769</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>34</v>
@@ -38042,7 +38041,7 @@
         <v>22</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="O12" s="10" t="s">
         <v>99</v>
@@ -38063,16 +38062,16 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="B13" s="58" t="s">
         <v>770</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="C13" s="100" t="s">
         <v>771</v>
       </c>
-      <c r="C13" s="100" t="s">
+      <c r="D13" s="5" t="s">
         <v>772</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>773</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>18</v>
@@ -38111,16 +38110,16 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="B14" s="58" t="s">
         <v>774</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="C14" s="7" t="s">
         <v>775</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>776</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>18</v>
@@ -38159,16 +38158,16 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="B15" s="58" t="s">
         <v>777</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="C15" s="7" t="s">
         <v>778</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>779</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>18</v>
@@ -38186,7 +38185,7 @@
         <v>22</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="O15" s="10" t="s">
         <v>99</v>
@@ -38207,16 +38206,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="B16" s="58" t="s">
         <v>780</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="C16" s="7" t="s">
         <v>781</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>782</v>
-      </c>
       <c r="D16" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>18</v>
@@ -38255,16 +38254,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="B17" s="58" t="s">
         <v>783</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="C17" s="7" t="s">
         <v>784</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>785</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>18</v>
@@ -38303,16 +38302,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="B18" s="58" t="s">
         <v>786</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="C18" s="7" t="s">
         <v>787</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>788</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
@@ -38363,16 +38362,16 @@
     </row>
     <row r="20">
       <c r="A20" s="65" t="s">
+        <v>788</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="7" t="s">
         <v>790</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>791</v>
-      </c>
       <c r="D20" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>34</v>
@@ -38390,7 +38389,7 @@
         <v>22</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="O20" s="10" t="s">
         <v>99</v>
@@ -38411,16 +38410,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>792</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="7" t="s">
         <v>793</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>794</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>795</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>18</v>
@@ -38459,16 +38458,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="7" t="s">
         <v>797</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>798</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>18</v>
@@ -38507,16 +38506,16 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="7" t="s">
         <v>800</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>801</v>
-      </c>
       <c r="D23" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -38555,16 +38554,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>802</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="7" t="s">
         <v>803</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>804</v>
-      </c>
       <c r="D24" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>18</v>
@@ -38603,16 +38602,16 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="7" t="s">
         <v>806</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>807</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -38651,16 +38650,16 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>808</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="7" t="s">
         <v>809</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>810</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>18</v>
@@ -38669,7 +38668,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="94" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="9">
@@ -38701,16 +38700,16 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>812</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C27" s="7" t="s">
         <v>813</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>814</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -38719,7 +38718,7 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="94" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="9">
@@ -38762,16 +38761,16 @@
     </row>
     <row r="29">
       <c r="A29" s="65" t="s">
+        <v>815</v>
+      </c>
+      <c r="B29" s="58" t="s">
         <v>816</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="C29" s="7" t="s">
         <v>817</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>818</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>34</v>
@@ -38780,7 +38779,7 @@
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="121" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="9">
@@ -38791,7 +38790,7 @@
         <v>22</v>
       </c>
       <c r="N29" s="122" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
@@ -38810,16 +38809,16 @@
     </row>
     <row r="30">
       <c r="A30" s="123" t="s">
+        <v>819</v>
+      </c>
+      <c r="B30" s="124" t="s">
         <v>820</v>
       </c>
-      <c r="B30" s="124" t="s">
+      <c r="C30" s="125" t="s">
         <v>821</v>
       </c>
-      <c r="C30" s="125" t="s">
+      <c r="D30" s="126" t="s">
         <v>822</v>
-      </c>
-      <c r="D30" s="126" t="s">
-        <v>823</v>
       </c>
       <c r="E30" s="126" t="s">
         <v>18</v>
@@ -38828,10 +38827,10 @@
       <c r="G30" s="127"/>
       <c r="H30" s="127"/>
       <c r="I30" s="121" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="J30" s="128" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K30" s="129">
         <v>44139.0</v>
@@ -38843,7 +38842,7 @@
         <v>294</v>
       </c>
       <c r="N30" s="122" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O30" s="131" t="s">
         <v>51</v>
@@ -38866,16 +38865,16 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
+        <v>824</v>
+      </c>
+      <c r="B31" s="58" t="s">
         <v>825</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="C31" s="7" t="s">
         <v>826</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>827</v>
-      </c>
       <c r="D31" s="114" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>18</v>
@@ -38912,16 +38911,16 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="B32" s="58" t="s">
         <v>828</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="C32" s="7" t="s">
         <v>829</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>830</v>
-      </c>
       <c r="D32" s="114" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>18</v>
@@ -43742,22 +43741,22 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>831</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>832</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>833</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -43792,22 +43791,22 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="7" t="s">
         <v>835</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>836</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -43824,7 +43823,7 @@
         <v>81</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -43842,22 +43841,22 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
+        <v>838</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>840</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>841</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -43874,7 +43873,7 @@
         <v>81</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -43892,22 +43891,22 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>843</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>844</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -43924,7 +43923,7 @@
         <v>81</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>

</xml_diff>

<commit_message>
300: fixed non-list iteration, added links to module pages
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/purpose_processing.xlsx
+++ b/documentation-generator/vocab_csv/purpose_processing.xlsx
@@ -2025,7 +2025,7 @@
     <t>The algorithmic logic applied or used</t>
   </si>
   <si>
-    <t>dpv:AutomationOfProcessing</t>
+    <t>dpv:ProcessingContext</t>
   </si>
   <si>
     <t>Algorithmic Logic is intended as a broad concept for explaining the use of algorithms and automated decisions making within Processing. To describe the actual algorithm, see the Algorithm concept.</t>
@@ -2040,9 +2040,6 @@
     <t>Processing that involves decision making</t>
   </si>
   <si>
-    <t>dpv:ProcessingContext</t>
-  </si>
-  <si>
     <t>AutomatedDecisionMaking</t>
   </si>
   <si>
@@ -2052,7 +2049,7 @@
     <t>Processing that involves automated decision making</t>
   </si>
   <si>
-    <t>dpv:DecisionMaking,dpv:AutomationOfProcessing</t>
+    <t>dpv:DecisionMaking</t>
   </si>
   <si>
     <t>Automated decision making can be defined as “the ability to make decisions by technological means without human involvement.” (“Guidelines on Automated individual decision-making and Profiling for the purposes of Regulation 2016/679 (wp251rev.01)”, 2018, p. 8)</t>
@@ -2183,6 +2180,9 @@
   </si>
   <si>
     <t>dpv:HumanInvolvementForInput</t>
+  </si>
+  <si>
+    <t>dpv:AutomationOfProcessing</t>
   </si>
   <si>
     <t>For example, an algorithm that takes inputs from humans and performs operations based on them</t>
@@ -27250,7 +27250,7 @@
         <v>44587.0</v>
       </c>
       <c r="L5" s="45">
-        <v>44727.0</v>
+        <v>45270.0</v>
       </c>
       <c r="M5" s="104" t="s">
         <v>23</v>
@@ -27288,7 +27288,7 @@
         <v>599</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E6" s="44" t="s">
         <v>590</v>
@@ -27327,16 +27327,16 @@
     </row>
     <row r="7">
       <c r="A7" s="104" t="s">
+        <v>600</v>
+      </c>
+      <c r="B7" s="105" t="s">
         <v>601</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="C7" s="90" t="s">
         <v>602</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="D7" s="44" t="s">
         <v>603</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>604</v>
       </c>
       <c r="E7" s="44" t="s">
         <v>590</v>
@@ -27345,7 +27345,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
       <c r="I7" s="44" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J7" s="96" t="s">
         <v>454</v>
@@ -27360,7 +27360,7 @@
         <v>23</v>
       </c>
       <c r="N7" s="104" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O7" s="46" t="s">
         <v>100</v>
@@ -27396,16 +27396,16 @@
     </row>
     <row r="9">
       <c r="A9" s="65" t="s">
+        <v>606</v>
+      </c>
+      <c r="B9" s="65" t="s">
+        <v>606</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>607</v>
       </c>
-      <c r="B9" s="65" t="s">
-        <v>607</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>608</v>
-      </c>
       <c r="D9" s="44" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E9" s="44" t="s">
         <v>590</v>
@@ -27442,26 +27442,26 @@
     </row>
     <row r="10">
       <c r="A10" s="44" t="s">
+        <v>608</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>608</v>
+      </c>
+      <c r="C10" s="44" t="s">
         <v>609</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>609</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>610</v>
       </c>
       <c r="D10" s="106"/>
       <c r="E10" s="106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="97" t="s">
+        <v>611</v>
+      </c>
+      <c r="J10" s="96" t="s">
         <v>612</v>
-      </c>
-      <c r="J10" s="96" t="s">
-        <v>613</v>
       </c>
       <c r="K10" s="45">
         <v>45270.0</v>
@@ -27490,23 +27490,23 @@
     </row>
     <row r="11">
       <c r="A11" s="44" t="s">
+        <v>613</v>
+      </c>
+      <c r="B11" s="44" t="s">
         <v>614</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="C11" s="44" t="s">
         <v>615</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>616</v>
       </c>
       <c r="D11" s="106"/>
       <c r="E11" s="106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="97" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="J11" s="20"/>
       <c r="K11" s="45">
@@ -27536,23 +27536,23 @@
     </row>
     <row r="12">
       <c r="A12" s="44" t="s">
+        <v>617</v>
+      </c>
+      <c r="B12" s="44" t="s">
         <v>618</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="C12" s="44" t="s">
         <v>619</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>620</v>
       </c>
       <c r="D12" s="106"/>
       <c r="E12" s="106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
       <c r="I12" s="97" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J12" s="20"/>
       <c r="K12" s="45">
@@ -27582,23 +27582,23 @@
     </row>
     <row r="13">
       <c r="A13" s="44" t="s">
+        <v>621</v>
+      </c>
+      <c r="B13" s="44" t="s">
         <v>622</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="C13" s="44" t="s">
         <v>623</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>624</v>
       </c>
       <c r="D13" s="106"/>
       <c r="E13" s="106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="97" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="45">
@@ -27628,23 +27628,23 @@
     </row>
     <row r="14">
       <c r="A14" s="44" t="s">
+        <v>624</v>
+      </c>
+      <c r="B14" s="44" t="s">
         <v>625</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="C14" s="44" t="s">
         <v>626</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>627</v>
       </c>
       <c r="D14" s="106"/>
       <c r="E14" s="106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
       <c r="I14" s="97" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="J14" s="20"/>
       <c r="K14" s="45">
@@ -27674,23 +27674,23 @@
     </row>
     <row r="15">
       <c r="A15" s="44" t="s">
+        <v>628</v>
+      </c>
+      <c r="B15" s="44" t="s">
         <v>629</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="C15" s="44" t="s">
         <v>630</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>631</v>
       </c>
       <c r="D15" s="106"/>
       <c r="E15" s="106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
       <c r="I15" s="97" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J15" s="20"/>
       <c r="K15" s="45">
@@ -27720,23 +27720,23 @@
     </row>
     <row r="16">
       <c r="A16" s="44" t="s">
+        <v>632</v>
+      </c>
+      <c r="B16" s="44" t="s">
         <v>633</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="C16" s="44" t="s">
         <v>634</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>635</v>
       </c>
       <c r="D16" s="106"/>
       <c r="E16" s="106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="97" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J16" s="20"/>
       <c r="K16" s="45">
@@ -27779,16 +27779,16 @@
     </row>
     <row r="18">
       <c r="A18" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="B18" s="44" t="s">
         <v>637</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="C18" s="90" t="s">
         <v>638</v>
       </c>
-      <c r="C18" s="90" t="s">
-        <v>639</v>
-      </c>
       <c r="D18" s="106" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E18" s="106" t="s">
         <v>590</v>
@@ -27797,7 +27797,7 @@
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="97" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J18" s="20"/>
       <c r="K18" s="45">
@@ -27829,19 +27829,19 @@
     </row>
     <row r="19">
       <c r="A19" s="44" t="s">
+        <v>640</v>
+      </c>
+      <c r="B19" s="44" t="s">
         <v>641</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="C19" s="90" t="s">
         <v>642</v>
       </c>
-      <c r="C19" s="90" t="s">
+      <c r="D19" s="106" t="s">
         <v>643</v>
       </c>
-      <c r="D19" s="106" t="s">
+      <c r="E19" s="106" t="s">
         <v>644</v>
-      </c>
-      <c r="E19" s="106" t="s">
-        <v>595</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
@@ -27893,7 +27893,7 @@
         <v>649</v>
       </c>
       <c r="E20" s="106" t="s">
-        <v>595</v>
+        <v>644</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -27945,7 +27945,7 @@
         <v>654</v>
       </c>
       <c r="E21" s="106" t="s">
-        <v>595</v>
+        <v>644</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -27995,7 +27995,7 @@
       </c>
       <c r="D22" s="107"/>
       <c r="E22" s="106" t="s">
-        <v>595</v>
+        <v>644</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
@@ -28043,7 +28043,7 @@
       </c>
       <c r="D23" s="107"/>
       <c r="E23" s="106" t="s">
-        <v>595</v>
+        <v>644</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
@@ -28089,7 +28089,7 @@
       </c>
       <c r="D24" s="107"/>
       <c r="E24" s="106" t="s">
-        <v>595</v>
+        <v>644</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -28149,7 +28149,7 @@
         <v>669</v>
       </c>
       <c r="D26" s="106" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E26" s="106" t="s">
         <v>590</v>
@@ -28673,7 +28673,7 @@
         <v>712</v>
       </c>
       <c r="D38" s="44" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E38" s="44" t="s">
         <v>590</v>
@@ -29004,7 +29004,7 @@
         <v>735</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E47" s="44" t="s">
         <v>590</v>
@@ -29024,7 +29024,7 @@
         <v>23</v>
       </c>
       <c r="N47" s="104" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O47" s="104" t="s">
         <v>51</v>
@@ -29156,7 +29156,7 @@
         <v>745</v>
       </c>
       <c r="D50" s="44" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="20"/>
@@ -29174,7 +29174,7 @@
         <v>290</v>
       </c>
       <c r="N50" s="104" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O50" s="43" t="s">
         <v>82</v>
@@ -29256,7 +29256,7 @@
         <v>752</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E53" s="44" t="s">
         <v>590</v>
@@ -29370,7 +29370,7 @@
         <v>23</v>
       </c>
       <c r="N55" s="104" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O55" s="104" t="s">
         <v>51</v>
@@ -29653,7 +29653,7 @@
       </c>
       <c r="D62" s="20"/>
       <c r="E62" s="26" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
@@ -29670,7 +29670,7 @@
         <v>23</v>
       </c>
       <c r="N62" s="104" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O62" s="104" t="s">
         <v>51</v>
@@ -29707,7 +29707,7 @@
         <v>787</v>
       </c>
       <c r="D64" s="44" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E64" s="44" t="s">
         <v>590</v>
@@ -34788,7 +34788,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>595</v>
+        <v>644</v>
       </c>
       <c r="F5" s="44" t="s">
         <v>431</v>
@@ -39135,7 +39135,7 @@
         <v>826</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E2" s="44" t="s">
         <v>590</v>
@@ -40274,7 +40274,7 @@
         <v>23</v>
       </c>
       <c r="N29" s="133" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O29" s="20"/>
       <c r="P29" s="20"/>
@@ -40324,7 +40324,7 @@
         <v>23</v>
       </c>
       <c r="N30" s="133" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O30" s="142" t="s">
         <v>51</v>

</xml_diff>